<commit_message>
ready for iteration 3
</commit_message>
<xml_diff>
--- a/prompt_engineering/prompt_column_anls.xlsx
+++ b/prompt_engineering/prompt_column_anls.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9588835-5D97-47F9-A72C-4CCB6D0FF53A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44032436-4F6B-4F87-82BF-A50FB9413BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>Examen</t>
   </si>
@@ -90,6 +90,21 @@
   </si>
   <si>
     <t>% d'ADN muté</t>
+  </si>
+  <si>
+    <t>gemma3 4b</t>
+  </si>
+  <si>
+    <t>qwen</t>
+  </si>
+  <si>
+    <t>qwen 3B</t>
+  </si>
+  <si>
+    <t>gemma</t>
+  </si>
+  <si>
+    <t>llama</t>
   </si>
 </sst>
 </file>
@@ -411,20 +426,27 @@
   <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="6.21875" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="0" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="6.33203125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="6" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="0" hidden="1" customWidth="1"/>
-    <col min="16" max="18" width="0" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="5.88671875" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="7.88671875" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="6" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="5.44140625" customWidth="1"/>
+    <col min="17" max="17" width="8.44140625" customWidth="1"/>
+    <col min="18" max="18" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
@@ -859,6 +881,29 @@
         <v>16</v>
       </c>
     </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L12" t="s">
+        <v>22</v>
+      </c>
+      <c r="M12" t="s">
+        <v>19</v>
+      </c>
+    </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>0</v>
@@ -867,9 +912,6 @@
         <f t="shared" ref="B13:B19" si="4">AVERAGE(C13:E13)</f>
         <v>1</v>
       </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
       <c r="D13">
         <v>1</v>
       </c>
@@ -891,9 +933,6 @@
         <v>1</v>
       </c>
       <c r="K13">
-        <v>1</v>
-      </c>
-      <c r="L13">
         <v>1</v>
       </c>
       <c r="M13">
@@ -908,9 +947,6 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
       <c r="D14">
         <v>1</v>
       </c>
@@ -929,13 +965,10 @@
       </c>
       <c r="J14">
         <f t="shared" si="6"/>
-        <v>0.95833333333333337</v>
+        <v>1</v>
       </c>
       <c r="K14">
         <v>1</v>
-      </c>
-      <c r="L14">
-        <v>0.875</v>
       </c>
       <c r="M14">
         <v>1</v>
@@ -947,10 +980,7 @@
       </c>
       <c r="B15">
         <f t="shared" si="4"/>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -960,26 +990,23 @@
       </c>
       <c r="F15">
         <f t="shared" si="5"/>
-        <v>0.5</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="H15">
         <v>1</v>
       </c>
       <c r="J15">
         <f t="shared" si="6"/>
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="K15">
         <v>1</v>
       </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
       <c r="M15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
@@ -988,10 +1015,7 @@
       </c>
       <c r="B16">
         <f t="shared" si="4"/>
-        <v>0.91133333333333333</v>
-      </c>
-      <c r="C16">
-        <v>0.75</v>
+        <v>0.99199999999999999</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1011,13 +1035,10 @@
       </c>
       <c r="J16">
         <f t="shared" si="6"/>
-        <v>0.95833333333333337</v>
+        <v>1</v>
       </c>
       <c r="K16">
         <v>1</v>
-      </c>
-      <c r="L16">
-        <v>0.875</v>
       </c>
       <c r="M16">
         <v>1</v>
@@ -1029,10 +1050,7 @@
       </c>
       <c r="B17">
         <f t="shared" si="4"/>
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="C17">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1052,13 +1070,10 @@
       </c>
       <c r="J17">
         <f t="shared" si="6"/>
-        <v>0.95833333333333337</v>
+        <v>1</v>
       </c>
       <c r="K17">
         <v>1</v>
-      </c>
-      <c r="L17">
-        <v>0.875</v>
       </c>
       <c r="M17">
         <v>1</v>
@@ -1070,10 +1085,7 @@
       </c>
       <c r="B18">
         <f t="shared" si="4"/>
-        <v>0.93900000000000006</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
+        <v>0.90850000000000009</v>
       </c>
       <c r="D18">
         <v>0.9</v>
@@ -1093,13 +1105,10 @@
       </c>
       <c r="J18">
         <f t="shared" si="6"/>
-        <v>0.94166666666666676</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="K18">
         <v>0.95</v>
-      </c>
-      <c r="L18">
-        <v>0.875</v>
       </c>
       <c r="M18">
         <v>1</v>
@@ -1111,10 +1120,7 @@
       </c>
       <c r="B19">
         <f t="shared" si="4"/>
-        <v>0.6</v>
-      </c>
-      <c r="C19">
-        <v>0.5</v>
+        <v>0.65</v>
       </c>
       <c r="D19">
         <v>0.65</v>
@@ -1134,13 +1140,10 @@
       </c>
       <c r="J19">
         <f t="shared" si="6"/>
-        <v>0.69899999999999995</v>
+        <v>0.73599999999999999</v>
       </c>
       <c r="K19">
         <v>0.75</v>
-      </c>
-      <c r="L19">
-        <v>0.625</v>
       </c>
       <c r="M19">
         <v>0.72199999999999998</v>

</xml_diff>